<commit_message>
update test cases excel sheet with correct file
</commit_message>
<xml_diff>
--- a/fundamentals-test-cases.xlsx
+++ b/fundamentals-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudau\OneDrive\Desktop\CPR\Final Project Summer 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F005B1-E2BA-49BF-BED1-E1A186A35DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF1D6A9-65E2-49C8-9F64-8712FE79AC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,7 +767,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>Comments</t>
   </si>
@@ -932,8 +932,41 @@
     <t>The length of 'd' is 1 characters</t>
   </si>
   <si>
-    <t>User enters "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula."
-input: "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula."</t>
+    <t>- Entering an empty string</t>
+  </si>
+  <si>
+    <t>User enters an empty string as the string 
+Input: An empty string</t>
+  </si>
+  <si>
+    <t>The length of '' is 0 characters</t>
+  </si>
+  <si>
+    <t>The length of 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula' is 79 characters long</t>
+  </si>
+  <si>
+    <t>- Entering string 80 characters long</t>
+  </si>
+  <si>
+    <t>User enters "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nunc id leo massa duis." as the string
+input: "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nunc id leo massa duis."</t>
+  </si>
+  <si>
+    <t>User enters "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula" as the string
+input: "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula"</t>
+  </si>
+  <si>
+    <t>The length of 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nunc id leo massa duis.' is 79 characters long</t>
+  </si>
+  <si>
+    <t>The length of 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer lacinia ligula.' is 78 characters long
+Type not empty string (q- to quit):
+The length of '' is 0 characters</t>
+  </si>
+  <si>
+    <t>The length of 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nunc id leo massa duis.' is 78 characters long
+Type not empty string (q- to quit):
+The length of '.' is 1 characters</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1275,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1346,6 +1379,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1652,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1914,7 @@
       <c r="B12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="17" t="s">
@@ -1900,7 +1936,7 @@
       <c r="C13" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="17"/>
@@ -1909,37 +1945,65 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" s="16" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="16" customFormat="1" ht="132" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="14"/>
+    <row r="16" spans="1:7" s="16" customFormat="1" ht="132" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>2</v>
+      </c>
       <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" s="16" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update excel sheet and testing text file with V3 requirements
</commit_message>
<xml_diff>
--- a/fundamentals-test-cases.xlsx
+++ b/fundamentals-test-cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudau\OneDrive\Desktop\CPR\Final Project Summer 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudau\OneDrive\Desktop\CPR\Final Project Summer 2022\V2 Final Project\cpr101-finalproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF1D6A9-65E2-49C8-9F64-8712FE79AC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63185A57-B423-40AD-8EA7-562B93DC279E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3132" yWindow="1344" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamentals" sheetId="3" r:id="rId1"/>
@@ -767,7 +767,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
   <si>
     <t>Comments</t>
   </si>
@@ -918,10 +918,6 @@
     <t>+ Normal test case: Entering a typical sentence as the string</t>
   </si>
   <si>
-    <t>User enters "d"
-Input: "orange man" and 0</t>
-  </si>
-  <si>
     <t>User enters "hello world! This is my program!" as the string
 Input: "hello world! This is my program!"</t>
   </si>
@@ -967,6 +963,63 @@
     <t>The length of 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Nunc id leo massa duis.' is 78 characters long
 Type not empty string (q- to quit):
 The length of '.' is 1 characters</t>
+  </si>
+  <si>
+    <t>User enters the string "The quick brown fox jumps over the lazy dog" as the string
+Input: "The quick brown fox jumps over the lazy dog"</t>
+  </si>
+  <si>
+    <t>New destination string is 'The quick brown fox jumps over the lazy dog'</t>
+  </si>
+  <si>
+    <t>User enters "d"
+Input: "d"</t>
+  </si>
+  <si>
+    <t>User enters "p"
+Input: "p"</t>
+  </si>
+  <si>
+    <t>New destination string is 'p'</t>
+  </si>
+  <si>
+    <t>+ Entering a string 1 character long</t>
+  </si>
+  <si>
+    <t>User enters an empty string as the string 
+Input: ""</t>
+  </si>
+  <si>
+    <t>New destination string is ''</t>
+  </si>
+  <si>
+    <t>User enters "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec at lorem tellus." as the string
+Input: "Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec at lorem tellus."</t>
+  </si>
+  <si>
+    <t>New destination string is 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec at lorem tellus.'</t>
+  </si>
+  <si>
+    <t>User enters "Pellentesque habitant morbi tristique senectus et netus et malesuada fames nunce" as the string
+Input: "Pellentesque habitant morbi tristique senectus et netus et malesuada fames nunce"</t>
+  </si>
+  <si>
+    <t>New destination string is 'Pellentesque habitant morbi tristique senectus et netus et malesuada fames nunc'</t>
+  </si>
+  <si>
+    <t>Recommended Fix: Clear the input buffer after the string is copied from the source to the destination</t>
+  </si>
+  <si>
+    <t>New destination string is 'Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec at lorem tellus'
+Destination string is reset to empty
+Type the source string (q - to quit) :
+New destination string is ''</t>
+  </si>
+  <si>
+    <t>New destination string is 'Pellentesque habitant morbi tristique senectus et netus et malesuada fames nun'
+Destination string is reset to empty
+Type the source string (q - to quit) :
+New destination string is 'e'</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1328,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1368,6 +1421,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1379,9 +1438,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1688,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1710,23 +1766,23 @@
       <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34" t="str">
+      <c r="C1" s="36" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1870,13 +1926,13 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="8" t="s">
         <v>5</v>
       </c>
@@ -1915,10 +1971,10 @@
         <v>38</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="14" t="s">
@@ -1927,17 +1983,17 @@
       <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="32" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>39</v>
+      <c r="C13" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="14" t="s">
@@ -1953,13 +2009,13 @@
         <v>36</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>2</v>
@@ -1971,13 +2027,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="14" t="s">
@@ -1986,20 +2042,20 @@
       <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:7" s="16" customFormat="1" ht="132" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="32" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="D16" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>2</v>
@@ -2016,13 +2072,13 @@
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="8" t="s">
         <v>5</v>
       </c>
@@ -2053,50 +2109,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+    <row r="20" spans="1:7" s="16" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="E20" s="17"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+    <row r="21" spans="1:7" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+    <row r="22" spans="1:7" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E22" s="17"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="14"/>
+    <row r="23" spans="1:7" s="16" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>2</v>
+      </c>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="21"/>
+    <row r="24" spans="1:7" s="16" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>

</xml_diff>